<commit_message>
replaced with original file
</commit_message>
<xml_diff>
--- a/VariantSurvival_package/R/metadata.xlsx
+++ b/VariantSurvival_package/R/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\mostafa\GeneTarget\GeneTarget\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahe9165/Documents/VariantSurvival/VariantSurvival_package/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0BE58-DE5C-4720-A66C-B7A7D3391F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EE50D3-F356-F347-83B2-3F0871128234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BDF8D68-BE9A-9E4A-A515-1221F880875C}"/>
+    <workbookView xWindow="9960" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{3BDF8D68-BE9A-9E4A-A515-1221F880875C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="101">
   <si>
     <t>Phenotype</t>
   </si>
@@ -399,7 +399,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -687,7 +687,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -695,18 +695,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005DD06C-617E-E24C-8013-5760C81D8236}">
-  <dimension ref="A1:X68"/>
+  <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="21" max="21" width="33.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -780,7 +781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -854,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -928,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1211,8 +1212,8 @@
       <c r="T7" t="s">
         <v>26</v>
       </c>
-      <c r="U7">
-        <v>584</v>
+      <c r="U7" t="s">
+        <v>21</v>
       </c>
       <c r="V7" t="s">
         <v>21</v>
@@ -1224,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1298,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1446,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1520,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1668,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1742,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1877,8 +1878,8 @@
       <c r="T16" t="s">
         <v>26</v>
       </c>
-      <c r="U16">
-        <v>254</v>
+      <c r="U16" t="s">
+        <v>21</v>
       </c>
       <c r="V16" t="s">
         <v>21</v>
@@ -1890,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2112,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2186,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2260,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2334,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2408,7 +2409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -2482,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -2630,7 +2631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2704,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2765,8 +2766,8 @@
       <c r="T28" t="s">
         <v>26</v>
       </c>
-      <c r="U28">
-        <v>254</v>
+      <c r="U28" t="s">
+        <v>21</v>
       </c>
       <c r="V28" t="s">
         <v>21</v>
@@ -2778,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2839,8 +2840,8 @@
       <c r="T29" t="s">
         <v>26</v>
       </c>
-      <c r="U29">
-        <v>365</v>
+      <c r="U29" t="s">
+        <v>21</v>
       </c>
       <c r="V29" t="s">
         <v>21</v>
@@ -2852,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -2926,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -3000,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -3074,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -3209,8 +3210,8 @@
       <c r="T34" t="s">
         <v>26</v>
       </c>
-      <c r="U34">
-        <v>4865</v>
+      <c r="U34" t="s">
+        <v>21</v>
       </c>
       <c r="V34" t="s">
         <v>21</v>
@@ -3222,7 +3223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -3296,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -3444,7 +3445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -3518,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -3579,8 +3580,8 @@
       <c r="T39" t="s">
         <v>26</v>
       </c>
-      <c r="U39">
-        <v>425</v>
+      <c r="U39" t="s">
+        <v>21</v>
       </c>
       <c r="V39" t="s">
         <v>21</v>
@@ -3592,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -3740,7 +3741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -3814,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3888,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -3962,7 +3963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -4036,7 +4037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -4110,7 +4111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -4184,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -4258,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -4332,7 +4333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -4406,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -4480,7 +4481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -4554,7 +4555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -4628,7 +4629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -4702,7 +4703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -4776,7 +4777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -4850,7 +4851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -4924,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -4998,7 +4999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -5072,7 +5073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -5146,7 +5147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -5220,7 +5221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>94</v>
       </c>
@@ -5294,7 +5295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>95</v>
       </c>
@@ -5368,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>96</v>
       </c>
@@ -5442,7 +5443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -5516,7 +5517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -5590,7 +5591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>99</v>
       </c>
@@ -5664,7 +5665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>100</v>
       </c>
@@ -5736,6 +5737,231 @@
       </c>
       <c r="X68" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U69">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U70">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U71">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U72">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U73">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U74">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U75">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U76">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U77">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U78">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U79">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="U80">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="81" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U81">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="82" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U82">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="83" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U83">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="84" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U84">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="85" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U85">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="86" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U86">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="87" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U87">
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="88" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U88">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="89" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U89">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="90" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U90">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="91" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U91">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="92" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U92">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="93" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U93">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="94" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U94">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="95" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U95">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="96" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U96">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="97" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U97">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="98" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U98">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="99" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U99">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="100" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U100">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="101" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U101">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="102" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U102">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="103" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U103">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="104" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U104">
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="105" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U105">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="106" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U106">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="107" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U107">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="108" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U108">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="109" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U109">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="110" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U110">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="111" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U111">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="112" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U112">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="113" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U113">
+        <v>910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>